<commit_message>
code refactoring, add invoices list for each client
</commit_message>
<xml_diff>
--- a/Server/Data/Clients.xlsx
+++ b/Server/Data/Clients.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomci\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomci\Desktop\Stock-Management-System\Server\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C5D9D9B-7E08-4772-BA4E-971AB9B78CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D64C1EE-4D41-4117-BFA5-3CEC89AC056D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7458622B-54A5-45D4-98DD-7F23A091CC51}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>Michael Johnson</t>
   </si>
   <si>
-    <t>michael.johnson@example.com555-567-8901</t>
-  </si>
-  <si>
     <t>Mary Wilson</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>nancy.young@example.com</t>
+  </si>
+  <si>
+    <t>michael.johnson@example.com</t>
   </si>
 </sst>
 </file>
@@ -275,10 +275,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -624,7 +623,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" activeCellId="1" sqref="C20 H9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,21 +634,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -682,74 +681,74 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>13</v>
+      <c r="B5" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" t="s">
         <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
       </c>
       <c r="C11" t="s">
         <v>2</v>
@@ -757,21 +756,21 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -779,10 +778,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -790,68 +789,68 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
-        <v>44</v>
-      </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
         <v>47</v>
       </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
       <c r="C19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>